<commit_message>
update exception case with alternate workflow
</commit_message>
<xml_diff>
--- a/data/jira/exception.xlsx
+++ b/data/jira/exception.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Workspace\report-aea-data-editor-2020\data\jira\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B7E8384-3B34-44E2-B726-54CD27D782FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8046C5-34A0-458F-A7DB-0CDB6E4E7AA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{F15A0B5B-C295-4E3A-8879-F4AA008B0E15}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>AEAREP-358</t>
   </si>
@@ -45,9 +45,6 @@
     <t>AEAREP-471</t>
   </si>
   <si>
-    <t>approved -&gt; Done</t>
-  </si>
-  <si>
     <t>AEAREP-819</t>
   </si>
   <si>
@@ -99,7 +96,16 @@
     <t>reason_not_submitted</t>
   </si>
   <si>
-    <t>status_change</t>
+    <t>AEAREP-645</t>
+  </si>
+  <si>
+    <t>AEAREP-707</t>
+  </si>
+  <si>
+    <t>status_change_deviated</t>
+  </si>
+  <si>
+    <t>Alternate Workflow</t>
   </si>
 </sst>
 </file>
@@ -451,27 +457,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADD3824D-05F7-4DB7-9A15-2624B10F345C}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
         <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -501,7 +508,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -509,32 +516,32 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -542,57 +549,79 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
         <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>